<commit_message>
Update output files for overviews after correcting row index value types.
</commit_message>
<xml_diff>
--- a/schedules/schedule_classes_overview.xlsx
+++ b/schedules/schedule_classes_overview.xlsx
@@ -785,10 +785,8 @@
         <v>3</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="AD3" t="n">
         <v>1</v>
@@ -883,10 +881,8 @@
         <v>2</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -983,10 +979,8 @@
         <v>4</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD5" t="n">
         <v>1</v>
@@ -1057,10 +1051,8 @@
         <v>4</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -1131,10 +1123,8 @@
         <v>5</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD7" t="n">
         <v>1</v>
@@ -1205,10 +1195,8 @@
         <v>1</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -1279,10 +1267,8 @@
         <v>1</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD9" t="n">
         <v>1</v>
@@ -1353,10 +1339,8 @@
         <v>11</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -1427,10 +1411,8 @@
         <v>2</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD11" t="n">
         <v>2</v>
@@ -1501,10 +1483,8 @@
         <v>2</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
@@ -1575,10 +1555,8 @@
         <v>4</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD13" t="n">
         <v>3</v>
@@ -2220,10 +2198,8 @@
         <v>4</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -2318,10 +2294,8 @@
         <v>8</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -2492,10 +2466,8 @@
         <v>1</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -2566,10 +2538,8 @@
         <v>4</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -2640,10 +2610,8 @@
         <v>4</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD8" t="n">
         <v>1</v>
@@ -2714,10 +2682,8 @@
         <v>3</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -2788,10 +2754,8 @@
         <v>2</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD10" t="n">
         <v>2</v>
@@ -2916,10 +2880,8 @@
         <v>34</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD12" t="n">
         <v>2</v>
@@ -3205,10 +3167,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -3303,10 +3263,8 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -3403,10 +3361,8 @@
         <v>3</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -3477,10 +3433,8 @@
         <v>1</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -3625,10 +3579,8 @@
         <v>5</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD7" t="n">
         <v>2</v>
@@ -3699,10 +3651,8 @@
         <v>2</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>101</v>
       </c>
       <c r="AD8" t="n">
         <v>1</v>
@@ -3773,10 +3723,8 @@
         <v>2</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD9" t="n">
         <v>1</v>
@@ -3847,10 +3795,8 @@
         <v>5</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -3921,10 +3867,8 @@
         <v>1</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -3995,10 +3939,8 @@
         <v>2</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD12" t="n">
         <v>1</v>
@@ -4069,10 +4011,8 @@
         <v>3</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -4143,10 +4083,8 @@
         <v>4</v>
       </c>
       <c r="AB14" s="1" t="n"/>
-      <c r="AC14" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC14" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD14" t="n">
         <v>2</v>
@@ -4291,10 +4229,8 @@
         <v>3</v>
       </c>
       <c r="AB16" s="1" t="n"/>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC16" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD16" t="n">
         <v>1</v>
@@ -4365,10 +4301,8 @@
         <v>1</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
@@ -4439,10 +4373,8 @@
         <v>1</v>
       </c>
       <c r="AB18" s="1" t="n"/>
-      <c r="AC18" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC18" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD18" t="n">
         <v>1</v>
@@ -5112,10 +5044,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -5310,10 +5240,8 @@
         <v>2</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -5384,10 +5312,8 @@
         <v>4</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -5458,10 +5384,8 @@
         <v>3</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD6" t="n">
         <v>2</v>
@@ -5532,10 +5456,8 @@
         <v>4</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -5606,10 +5528,8 @@
         <v>2</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD8" t="n">
         <v>1</v>
@@ -5680,10 +5600,8 @@
         <v>5</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD9" t="n">
         <v>2</v>
@@ -5754,10 +5672,8 @@
         <v>1</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD10" t="n">
         <v>1</v>
@@ -5828,10 +5744,8 @@
         <v>6</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -5902,10 +5816,8 @@
         <v>2</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD12" t="n">
         <v>2</v>
@@ -5976,10 +5888,8 @@
         <v>2</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -6198,10 +6108,8 @@
         <v>1</v>
       </c>
       <c r="AB16" s="1" t="n"/>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC16" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
@@ -6274,10 +6182,8 @@
         <v>45</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
@@ -6797,10 +6703,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="AD2" t="n">
         <v>1</v>
@@ -6895,10 +6799,8 @@
         <v>8</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD3" t="n">
         <v>3</v>
@@ -6995,10 +6897,8 @@
         <v>7</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -7069,10 +6969,8 @@
         <v>3</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>209</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>209</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -7217,10 +7115,8 @@
         <v>3</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -7291,10 +7187,8 @@
         <v>2</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -7365,10 +7259,8 @@
         <v>2</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD9" t="n">
         <v>1</v>
@@ -7439,10 +7331,8 @@
         <v>1</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -7513,10 +7403,8 @@
         <v>3</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -7661,10 +7549,8 @@
         <v>1</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD13" t="n">
         <v>2</v>
@@ -7735,10 +7621,8 @@
         <v>3</v>
       </c>
       <c r="AB14" s="1" t="n"/>
-      <c r="AC14" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC14" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD14" t="n">
         <v>2</v>
@@ -7809,10 +7693,8 @@
         <v>2</v>
       </c>
       <c r="AB15" s="1" t="n"/>
-      <c r="AC15" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC15" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD15" t="n">
         <v>1</v>
@@ -8430,10 +8312,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -8628,10 +8508,8 @@
         <v>2</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -8776,10 +8654,8 @@
         <v>2</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -8850,10 +8726,8 @@
         <v>3</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -8924,10 +8798,8 @@
         <v>3</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -8998,10 +8870,8 @@
         <v>2</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>209</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>209</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -9072,10 +8942,8 @@
         <v>3</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD10" t="n">
         <v>2</v>
@@ -9146,10 +9014,8 @@
         <v>1</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -9220,10 +9086,8 @@
         <v>2</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
@@ -9294,10 +9158,8 @@
         <v>2</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -9368,10 +9230,8 @@
         <v>5</v>
       </c>
       <c r="AB14" s="1" t="n"/>
-      <c r="AC14" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC14" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD14" t="n">
         <v>0</v>
@@ -9516,10 +9376,8 @@
         <v>8</v>
       </c>
       <c r="AB16" s="1" t="n"/>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC16" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD16" t="n">
         <v>2</v>
@@ -9590,10 +9448,8 @@
         <v>4</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD17" t="n">
         <v>2</v>
@@ -10209,10 +10065,8 @@
         <v>2</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -10307,10 +10161,8 @@
         <v>1</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -10407,10 +10259,8 @@
         <v>5</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD5" t="n">
         <v>1</v>
@@ -10481,10 +10331,8 @@
         <v>2</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -10555,10 +10403,8 @@
         <v>1</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -10629,10 +10475,8 @@
         <v>4</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD8" t="n">
         <v>1</v>
@@ -10703,10 +10547,8 @@
         <v>1</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD9" t="n">
         <v>2</v>
@@ -10777,10 +10619,8 @@
         <v>3</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD10" t="n">
         <v>1</v>
@@ -10851,10 +10691,8 @@
         <v>1</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD11" t="n">
         <v>3</v>
@@ -11268,10 +11106,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -11366,10 +11202,8 @@
         <v>4</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -11464,10 +11298,8 @@
         <v>1</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -11562,10 +11394,8 @@
         <v>3</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -11760,10 +11590,8 @@
         <v>2</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -11984,10 +11812,8 @@
         <v>20</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -12036,10 +11862,8 @@
         <v>20</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -12325,10 +12149,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -12521,10 +12343,8 @@
         <v>7</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -12621,10 +12441,8 @@
         <v>2</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -12769,10 +12587,8 @@
         <v>2</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -12843,10 +12659,8 @@
         <v>1</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -12993,10 +12807,8 @@
         <v>17</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -13406,10 +13218,8 @@
         <v>2</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -13504,10 +13314,8 @@
         <v>3</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -13604,10 +13412,8 @@
         <v>3</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -13678,10 +13484,8 @@
         <v>1</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -13752,10 +13556,8 @@
         <v>3</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -13826,10 +13628,8 @@
         <v>2</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -13900,10 +13700,8 @@
         <v>1</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -14052,10 +13850,8 @@
         <v>17</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -14367,10 +14163,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD2" t="n">
         <v>1</v>
@@ -14467,10 +14261,8 @@
         <v>2</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -14615,10 +14407,8 @@
         <v>2</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -14689,10 +14479,8 @@
         <v>2</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -14763,10 +14551,8 @@
         <v>3</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD7" t="n">
         <v>1</v>
@@ -14837,10 +14623,8 @@
         <v>1</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD8" t="n">
         <v>1</v>
@@ -14911,10 +14695,8 @@
         <v>1</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -14985,10 +14767,8 @@
         <v>1</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -15425,10 +15205,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>209</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>209</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -15523,10 +15301,8 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>101</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -15621,10 +15397,8 @@
         <v>7</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD4" t="n">
         <v>3</v>
@@ -15721,10 +15495,8 @@
         <v>2</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="AD5" t="n">
         <v>1</v>
@@ -15943,10 +15715,8 @@
         <v>5</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -16017,10 +15787,8 @@
         <v>3</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -16091,10 +15859,8 @@
         <v>3</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -16165,10 +15931,8 @@
         <v>4</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -16239,10 +16003,8 @@
         <v>3</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
@@ -16313,10 +16075,8 @@
         <v>13</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -16387,10 +16147,8 @@
         <v>1</v>
       </c>
       <c r="AB14" s="1" t="n"/>
-      <c r="AC14" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC14" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD14" t="n">
         <v>0</v>
@@ -16461,10 +16219,8 @@
         <v>2</v>
       </c>
       <c r="AB15" s="1" t="n"/>
-      <c r="AC15" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC15" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD15" t="n">
         <v>0</v>
@@ -16535,10 +16291,8 @@
         <v>2</v>
       </c>
       <c r="AB16" s="1" t="n"/>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC16" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD16" t="n">
         <v>3</v>
@@ -16609,10 +16363,8 @@
         <v>2</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
@@ -16757,10 +16509,8 @@
         <v>3</v>
       </c>
       <c r="AB19" s="1" t="n"/>
-      <c r="AC19" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC19" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD19" t="n">
         <v>2</v>
@@ -16831,10 +16581,8 @@
         <v>4</v>
       </c>
       <c r="AB20" s="1" t="n"/>
-      <c r="AC20" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC20" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD20" t="n">
         <v>0</v>
@@ -17510,10 +17258,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -17610,10 +17356,8 @@
         <v>3</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -17684,10 +17428,8 @@
         <v>2</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -17758,10 +17500,8 @@
         <v>2</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -17832,10 +17572,8 @@
         <v>2</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD6" t="n">
         <v>1</v>
@@ -18222,10 +17960,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="AD2" t="n">
         <v>3</v>
@@ -18737,10 +18473,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -18837,10 +18571,8 @@
         <v>2</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD3" t="n">
         <v>1</v>
@@ -18911,10 +18643,8 @@
         <v>3</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD4" t="n">
         <v>2</v>
@@ -18985,10 +18715,8 @@
         <v>1</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -19059,10 +18787,8 @@
         <v>2</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD6" t="n">
         <v>1</v>
@@ -19133,10 +18859,8 @@
         <v>2</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -19207,10 +18931,8 @@
         <v>1</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -19547,10 +19269,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD2" t="n">
         <v>1</v>
@@ -19645,10 +19365,8 @@
         <v>5</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -19743,10 +19461,8 @@
         <v>2</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>101</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -19991,10 +19707,8 @@
         <v>3</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD7" t="n">
         <v>3</v>
@@ -20065,10 +19779,8 @@
         <v>4</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -20139,10 +19851,8 @@
         <v>8</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD9" t="n">
         <v>1</v>
@@ -20213,10 +19923,8 @@
         <v>4</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -20287,10 +19995,8 @@
         <v>3</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -20361,10 +20067,8 @@
         <v>7</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
@@ -20435,10 +20139,8 @@
         <v>1</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -20509,10 +20211,8 @@
         <v>2</v>
       </c>
       <c r="AB14" s="1" t="n"/>
-      <c r="AC14" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC14" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD14" t="n">
         <v>0</v>
@@ -20583,10 +20283,8 @@
         <v>1</v>
       </c>
       <c r="AB15" s="1" t="n"/>
-      <c r="AC15" s="1" t="inlineStr">
-        <is>
-          <t>209</t>
-        </is>
+      <c r="AC15" s="1" t="n">
+        <v>209</v>
       </c>
       <c r="AD15" t="n">
         <v>1</v>
@@ -20657,10 +20355,8 @@
         <v>2</v>
       </c>
       <c r="AB16" s="1" t="n"/>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC16" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
@@ -20731,10 +20427,8 @@
         <v>8</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD17" t="n">
         <v>1</v>
@@ -20879,10 +20573,8 @@
         <v>3</v>
       </c>
       <c r="AB19" s="1" t="n"/>
-      <c r="AC19" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC19" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD19" t="n">
         <v>0</v>
@@ -20955,10 +20647,8 @@
         <v>61</v>
       </c>
       <c r="AB20" s="1" t="n"/>
-      <c r="AC20" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC20" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD20" t="n">
         <v>1</v>
@@ -21530,10 +21220,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD2" t="n">
         <v>3</v>
@@ -21628,10 +21316,8 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -21726,10 +21412,8 @@
         <v>9</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>209</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>209</v>
       </c>
       <c r="AD4" t="n">
         <v>1</v>
@@ -21826,10 +21510,8 @@
         <v>8</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -21900,10 +21582,8 @@
         <v>3</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -21974,10 +21654,8 @@
         <v>3</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -22048,10 +21726,8 @@
         <v>4</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD8" t="n">
         <v>2</v>
@@ -22122,10 +21798,8 @@
         <v>5</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -22196,10 +21870,8 @@
         <v>2</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>101</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -22270,10 +21942,8 @@
         <v>3</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD11" t="n">
         <v>1</v>
@@ -22418,10 +22088,8 @@
         <v>2</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD13" t="n">
         <v>3</v>
@@ -22714,10 +22382,8 @@
         <v>1</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
@@ -22788,10 +22454,8 @@
         <v>2</v>
       </c>
       <c r="AB18" s="1" t="n"/>
-      <c r="AC18" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC18" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD18" t="n">
         <v>0</v>
@@ -22864,10 +22528,8 @@
         <v>58</v>
       </c>
       <c r="AB19" s="1" t="n"/>
-      <c r="AC19" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC19" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD19" t="n">
         <v>0</v>
@@ -23459,10 +23121,8 @@
         <v>4</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -23557,10 +23217,8 @@
         <v>3</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD4" t="n">
         <v>2</v>
@@ -23657,10 +23315,8 @@
         <v>4</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -23805,10 +23461,8 @@
         <v>3</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -23879,10 +23533,8 @@
         <v>5</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD8" t="n">
         <v>2</v>
@@ -23953,10 +23605,8 @@
         <v>8</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -24029,10 +23679,8 @@
         <v>34</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -24079,10 +23727,8 @@
         <v>1</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -24394,10 +24040,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -24492,10 +24136,8 @@
         <v>4</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -24590,10 +24232,8 @@
         <v>3</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD4" t="n">
         <v>1</v>
@@ -24690,10 +24330,8 @@
         <v>1</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -24764,10 +24402,8 @@
         <v>3</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD6" t="n">
         <v>2</v>
@@ -24838,10 +24474,8 @@
         <v>4</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -24912,10 +24546,8 @@
         <v>7</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD8" t="n">
         <v>1</v>
@@ -25060,10 +24692,8 @@
         <v>3</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -25134,10 +24764,8 @@
         <v>2</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -25282,10 +24910,8 @@
         <v>3</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -25430,10 +25056,8 @@
         <v>1</v>
       </c>
       <c r="AB15" s="1" t="n"/>
-      <c r="AC15" s="1" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="AC15" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="AD15" t="n">
         <v>0</v>
@@ -25504,10 +25128,8 @@
         <v>8</v>
       </c>
       <c r="AB16" s="1" t="n"/>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
+      <c r="AC16" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
@@ -25578,10 +25200,8 @@
         <v>2</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD17" t="n">
         <v>4</v>
@@ -25652,10 +25272,8 @@
         <v>9</v>
       </c>
       <c r="AB18" s="1" t="n"/>
-      <c r="AC18" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC18" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD18" t="n">
         <v>0</v>
@@ -25726,10 +25344,8 @@
         <v>2</v>
       </c>
       <c r="AB19" s="1" t="n"/>
-      <c r="AC19" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC19" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD19" t="n">
         <v>2</v>
@@ -26469,10 +26085,8 @@
         <v>3</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -26567,10 +26181,8 @@
         <v>1</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -26667,10 +26279,8 @@
         <v>3</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -26741,10 +26351,8 @@
         <v>2</v>
       </c>
       <c r="AB7" s="1" t="n"/>
-      <c r="AC7" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC7" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -26815,10 +26423,8 @@
         <v>16</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD8" t="n">
         <v>1</v>
@@ -26889,10 +26495,8 @@
         <v>3</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD9" t="n">
         <v>1</v>
@@ -26963,10 +26567,8 @@
         <v>1</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD10" t="n">
         <v>2</v>
@@ -27185,10 +26787,8 @@
         <v>2</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>208</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="AD13" t="n">
         <v>1</v>
@@ -27259,10 +26859,8 @@
         <v>4</v>
       </c>
       <c r="AB14" s="1" t="n"/>
-      <c r="AC14" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC14" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD14" t="n">
         <v>0</v>
@@ -27333,10 +26931,8 @@
         <v>5</v>
       </c>
       <c r="AB15" s="1" t="n"/>
-      <c r="AC15" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC15" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD15" t="n">
         <v>8</v>
@@ -27407,10 +27003,8 @@
         <v>2</v>
       </c>
       <c r="AB16" s="1" t="n"/>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC16" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
@@ -27481,10 +27075,8 @@
         <v>1</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD17" t="n">
         <v>1</v>
@@ -27555,10 +27147,8 @@
         <v>8</v>
       </c>
       <c r="AB18" s="1" t="n"/>
-      <c r="AC18" s="1" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="AC18" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="AD18" t="n">
         <v>1</v>
@@ -28048,10 +27638,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -28146,10 +27734,8 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -28342,10 +27928,8 @@
         <v>2</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD5" t="n">
         <v>1</v>
@@ -28442,10 +28026,8 @@
         <v>3</v>
       </c>
       <c r="AB6" s="1" t="n"/>
-      <c r="AC6" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC6" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -28590,10 +28172,8 @@
         <v>4</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD8" t="n">
         <v>2</v>
@@ -28738,10 +28318,8 @@
         <v>3</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>202</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="AD10" t="n">
         <v>2</v>
@@ -28812,10 +28390,8 @@
         <v>1</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD11" t="n">
         <v>1</v>
@@ -28886,10 +28462,8 @@
         <v>1</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>101</v>
       </c>
       <c r="AD12" t="n">
         <v>2</v>
@@ -28960,10 +28534,8 @@
         <v>6</v>
       </c>
       <c r="AB13" s="1" t="n"/>
-      <c r="AC13" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC13" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD13" t="n">
         <v>1</v>
@@ -29108,10 +28680,8 @@
         <v>4</v>
       </c>
       <c r="AB15" s="1" t="n"/>
-      <c r="AC15" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC15" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD15" t="n">
         <v>0</v>
@@ -29182,10 +28752,8 @@
         <v>1</v>
       </c>
       <c r="AB16" s="1" t="n"/>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="AC16" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
@@ -29256,10 +28824,8 @@
         <v>3</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>210</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
@@ -29330,10 +28896,8 @@
         <v>14</v>
       </c>
       <c r="AB18" s="1" t="n"/>
-      <c r="AC18" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC18" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD18" t="n">
         <v>0</v>
@@ -29404,10 +28968,8 @@
         <v>2</v>
       </c>
       <c r="AB19" s="1" t="n"/>
-      <c r="AC19" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC19" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD19" t="n">
         <v>0</v>
@@ -29901,10 +29463,8 @@
           <t>sala</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
+      <c r="AC2" s="1" t="n">
+        <v>101</v>
       </c>
       <c r="AD2" t="n">
         <v>2</v>
@@ -29999,10 +29559,8 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="n"/>
-      <c r="AC3" s="1" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
+      <c r="AC3" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="AD3" t="n">
         <v>1</v>
@@ -30097,10 +29655,8 @@
         <v>2</v>
       </c>
       <c r="AB4" s="1" t="n"/>
-      <c r="AC4" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="AC4" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -30197,10 +29753,8 @@
         <v>3</v>
       </c>
       <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="AC5" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -30419,10 +29973,8 @@
         <v>6</v>
       </c>
       <c r="AB8" s="1" t="n"/>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>207</t>
-        </is>
+      <c r="AC8" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="AD8" t="n">
         <v>2</v>
@@ -30493,10 +30045,8 @@
         <v>1</v>
       </c>
       <c r="AB9" s="1" t="n"/>
-      <c r="AC9" s="1" t="inlineStr">
-        <is>
-          <t>203</t>
-        </is>
+      <c r="AC9" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="AD9" t="n">
         <v>1</v>
@@ -30567,10 +30117,8 @@
         <v>6</v>
       </c>
       <c r="AB10" s="1" t="n"/>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+      <c r="AC10" s="1" t="n">
+        <v>102</v>
       </c>
       <c r="AD10" t="n">
         <v>2</v>
@@ -30641,10 +30189,8 @@
         <v>9</v>
       </c>
       <c r="AB11" s="1" t="n"/>
-      <c r="AC11" s="1" t="inlineStr">
-        <is>
-          <t>112</t>
-        </is>
+      <c r="AC11" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -30715,10 +30261,8 @@
         <v>1</v>
       </c>
       <c r="AB12" s="1" t="n"/>
-      <c r="AC12" s="1" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="AC12" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
@@ -30937,10 +30481,8 @@
         <v>2</v>
       </c>
       <c r="AB15" s="1" t="n"/>
-      <c r="AC15" s="1" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
+      <c r="AC15" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="AD15" t="n">
         <v>1</v>
@@ -31085,10 +30627,8 @@
         <v>2</v>
       </c>
       <c r="AB17" s="1" t="n"/>
-      <c r="AC17" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="AC17" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
@@ -31233,10 +30773,8 @@
         <v>3</v>
       </c>
       <c r="AB19" s="1" t="n"/>
-      <c r="AC19" s="1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
+      <c r="AC19" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="AD19" t="n">
         <v>0</v>
@@ -31307,10 +30845,8 @@
         <v>1</v>
       </c>
       <c r="AB20" s="1" t="n"/>
-      <c r="AC20" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="AC20" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="AD20" t="n">
         <v>0</v>
@@ -31381,10 +30917,8 @@
         <v>2</v>
       </c>
       <c r="AB21" s="1" t="n"/>
-      <c r="AC21" s="1" t="inlineStr">
-        <is>
-          <t>116</t>
-        </is>
+      <c r="AC21" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="AD21" t="n">
         <v>0</v>
@@ -31455,10 +30989,8 @@
         <v>2</v>
       </c>
       <c r="AB22" s="1" t="n"/>
-      <c r="AC22" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AC22" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AD22" t="n">
         <v>0</v>

</xml_diff>